<commit_message>
Final Code By team 12
</commit_message>
<xml_diff>
--- a/Team_12_LMS_Oct_2024/src/test/resources/Team_12_data_sheet.xlsx
+++ b/Team_12_LMS_Oct_2024/src/test/resources/Team_12_data_sheet.xlsx
@@ -1,21 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28025"/>
-  <workbookPr defaultThemeVersion="202300"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Varkha\Team 12 LMS Selenium\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{2D387F69-E994-4F61-9390-198CE67AD389}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="7" rupBuild="14420"/>
+  <workbookPr/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{93D8DA34-5D16-4F9D-819A-CF4C3A394DAF}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="19770" windowHeight="6180"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="152511"/>
+  <oleSize ref="A1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -35,15 +30,44 @@
 </workbook>
 </file>
 
+<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
+  <si>
+    <t>Name</t>
+  </si>
+  <si>
+    <t>Testingchatbot</t>
+  </si>
+  <si>
+    <t>Batch 03</t>
+  </si>
+  <si>
+    <t>By Program Name</t>
+  </si>
+  <si>
+    <t>Learning</t>
+  </si>
+  <si>
+    <t>Testing</t>
+  </si>
+</sst>
+</file>
+
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <fonts count="2">
     <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Aptos Narrow"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FF2A00FF"/>
+      <name val="Consolas"/>
+      <family val="3"/>
     </font>
   </fonts>
   <fills count="2">
@@ -66,8 +90,9 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -401,13 +426,47 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2AE81B33-BD4E-4FBC-AB49-8DD02757C374}">
-  <dimension ref="A1"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:A6"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A6" sqref="A6"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
-  <sheetData/>
+  <sheetFormatPr defaultRowHeight="14.25"/>
+  <sheetData>
+    <row r="1" spans="1:1">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1" ht="15.75">
+      <c r="A2" s="1" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:1" ht="15.75">
+      <c r="A3" s="1" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="4" spans="1:1" ht="15.75">
+      <c r="A4" s="1" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="5" spans="1:1" ht="15.75">
+      <c r="A5" s="1" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="6" spans="1:1" ht="15.75">
+      <c r="A6" s="1" t="s">
+        <v>5</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>